<commit_message>
Merge fnuciona con casos de prueba específicos, falta contemplar grupos de tamaño impar
</commit_message>
<xml_diff>
--- a/Array Merge.xlsx
+++ b/Array Merge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\solid\Desktop\ITC\Semestre3\Estructura Datos\Parcial4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E0F7D2A-E157-4948-B6D8-ACA2394B241E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0242217E-1E74-4025-925C-3D3D05D72B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D027E261-0996-4E73-9EA8-3C78A974A5B2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>i</t>
   </si>
@@ -47,15 +47,23 @@
     <t>Tamaño de grupos = 1</t>
   </si>
   <si>
-    <t>Tamaño de grupos = 2</t>
+    <t>Lim Index grupo = 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -195,11 +203,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,10 +241,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -243,7 +267,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +276,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,9 +304,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9999"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFCCFFFF"/>
-      <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
   <extLst>
@@ -576,151 +619,189 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1F7E58-B7CD-4169-A9E1-085807763DA9}">
   <dimension ref="C1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="18" width="5.81640625" customWidth="1"/>
-    <col min="19" max="19" width="6" style="24" customWidth="1"/>
+    <col min="19" max="19" width="6" style="19" customWidth="1"/>
     <col min="20" max="20" width="6.1796875" customWidth="1"/>
     <col min="21" max="21" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="9">
+      <c r="C2" s="5">
         <v>206</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="7">
         <v>298</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="6">
         <v>61</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="7">
         <v>68</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="6">
         <v>117</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="7">
         <v>157</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="6">
         <v>229</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="7">
         <v>63</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="6">
         <v>288</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="7">
         <v>184</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="6">
         <v>250</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="7">
         <v>218</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="6">
         <v>90</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="7">
         <v>296</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="6">
         <v>120</v>
       </c>
-      <c r="R2" s="11">
+      <c r="R2" s="7">
         <v>65</v>
       </c>
-      <c r="S2" s="25">
+      <c r="S2" s="20">
         <v>245</v>
       </c>
     </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C3" s="18">
+        <v>0</v>
+      </c>
+      <c r="D3" s="18">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18">
+        <v>2</v>
+      </c>
+      <c r="F3" s="18">
+        <v>3</v>
+      </c>
+      <c r="G3" s="18">
+        <v>4</v>
+      </c>
+      <c r="H3" s="18">
+        <v>5</v>
+      </c>
+      <c r="I3" s="18">
+        <v>6</v>
+      </c>
+      <c r="J3" s="18">
+        <v>7</v>
+      </c>
+    </row>
     <row r="4" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="7">
+      <c r="C5" s="23">
         <v>206</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="23">
         <v>61</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="23">
         <v>117</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="25">
         <v>229</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="25">
         <v>288</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="25">
         <v>250</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="25">
         <v>90</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="25">
         <v>120</v>
       </c>
-      <c r="K5" s="6">
-        <v>245</v>
-      </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
     </row>
     <row r="6" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F6" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26" t="s">
         <v>1</v>
       </c>
+      <c r="M6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="7">
+      <c r="C7" s="23">
         <v>298</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="23">
         <v>68</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="23">
         <v>157</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="14">
         <v>63</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="14">
         <v>184</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="14">
         <v>218</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="14">
         <v>296</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="14">
         <v>65</v>
       </c>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    </row>
+    <row r="8" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8" s="28"/>
+    </row>
     <row r="9" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="2">
         <v>206</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="27">
         <v>298</v>
       </c>
       <c r="E9" s="3">
@@ -759,67 +840,63 @@
       <c r="P9" s="3">
         <v>296</v>
       </c>
-      <c r="Q9" s="3">
-        <v>65</v>
-      </c>
-      <c r="R9" s="3">
-        <v>120</v>
-      </c>
-      <c r="S9" s="25">
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="20">
         <v>245</v>
       </c>
     </row>
     <row r="12" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="9">
+      <c r="C13" s="5">
         <v>206</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <v>298</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="7">
         <v>61</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="7">
         <v>68</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="6">
         <v>117</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="6">
         <v>157</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="7">
         <v>63</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="7">
         <v>229</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="6">
         <v>184</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="6">
         <v>288</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="7">
         <v>218</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="7">
         <v>250</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="6">
         <v>90</v>
       </c>
-      <c r="P13" s="10">
+      <c r="P13" s="6">
         <v>296</v>
       </c>
-      <c r="Q13" s="11">
+      <c r="Q13" s="7">
         <v>65</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="7">
         <v>120</v>
       </c>
-      <c r="S13" s="25">
+      <c r="S13" s="20">
         <v>245</v>
       </c>
     </row>
@@ -836,31 +913,28 @@
       <c r="F15" s="1">
         <v>3</v>
       </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
+      <c r="G15" s="30"/>
       <c r="H15" s="1">
         <v>5</v>
       </c>
-      <c r="I15" s="1">
-        <v>6</v>
-      </c>
+      <c r="I15" s="30"/>
       <c r="J15" s="1">
         <v>7</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="30">
         <v>8</v>
       </c>
-      <c r="N15" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
     </row>
     <row r="16" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E16" t="s">
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>0</v>
       </c>
     </row>
@@ -889,221 +963,225 @@
       <c r="J17" s="4">
         <v>296</v>
       </c>
-      <c r="K17" s="18">
-        <v>245</v>
-      </c>
-      <c r="L17" s="19"/>
+      <c r="L17" s="15"/>
+      <c r="N17" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
     </row>
     <row r="18" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="14"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="14" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="N18" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
     </row>
     <row r="19" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="13">
+      <c r="C19" s="29">
         <v>61</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="8">
         <v>68</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="9">
         <v>63</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="12">
         <v>229</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="9">
         <v>218</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="12">
         <v>250</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="9">
         <v>65</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="12">
         <v>120</v>
       </c>
-      <c r="K19" s="21">
-        <v>0</v>
-      </c>
-      <c r="L19" s="20"/>
+      <c r="L19" s="16"/>
     </row>
     <row r="21" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="9">
+      <c r="C22" s="5">
         <v>61</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <v>68</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>206</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="6">
         <v>298</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="7">
         <v>63</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="7">
         <v>117</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="7">
         <v>157</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="7">
         <v>229</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="6">
         <v>184</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="6">
         <v>218</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="6">
         <v>250</v>
       </c>
-      <c r="N22" s="10">
+      <c r="N22" s="6">
         <v>288</v>
       </c>
-      <c r="O22" s="11">
-        <v>65</v>
-      </c>
-      <c r="P22" s="11">
-        <v>90</v>
-      </c>
-      <c r="Q22" s="11">
-        <v>120</v>
-      </c>
-      <c r="R22" s="11">
-        <v>296</v>
-      </c>
-      <c r="S22" s="25">
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="20">
         <v>245</v>
       </c>
     </row>
     <row r="24" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="25" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="9">
+      <c r="C25" s="5">
         <v>61</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="6">
         <v>63</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="6">
         <v>68</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="6">
         <v>117</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="6">
         <v>157</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="6">
         <v>206</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="6">
         <v>229</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="6">
         <v>298</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="17">
         <v>65</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="17">
         <v>90</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="17">
         <v>120</v>
       </c>
-      <c r="N25" s="22">
+      <c r="N25" s="17">
         <v>184</v>
       </c>
-      <c r="O25" s="22">
+      <c r="O25" s="17">
         <v>218</v>
       </c>
-      <c r="P25" s="22">
+      <c r="P25" s="17">
         <v>250</v>
       </c>
-      <c r="Q25" s="22">
+      <c r="Q25" s="17">
         <v>288</v>
       </c>
-      <c r="R25" s="22">
+      <c r="R25" s="17">
         <v>296</v>
       </c>
-      <c r="S25" s="26">
+      <c r="S25" s="21">
         <v>245</v>
       </c>
     </row>
     <row r="27" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="28" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C28" s="9">
+      <c r="C28" s="5">
         <v>61</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="6">
         <v>63</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="6">
         <v>65</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="6">
         <v>68</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="6">
         <v>90</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="6">
         <v>117</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="6">
         <v>120</v>
       </c>
-      <c r="J28" s="10">
+      <c r="J28" s="6">
         <v>157</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="6">
         <v>184</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="6">
         <v>206</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="6">
         <v>218</v>
       </c>
-      <c r="N28" s="10">
+      <c r="N28" s="6">
         <v>229</v>
       </c>
-      <c r="O28" s="10">
+      <c r="O28" s="6">
         <v>250</v>
       </c>
-      <c r="P28" s="10">
+      <c r="P28" s="6">
         <v>288</v>
       </c>
-      <c r="Q28" s="10">
+      <c r="Q28" s="6">
         <v>296</v>
       </c>
-      <c r="R28" s="10">
+      <c r="R28" s="6">
         <v>298</v>
       </c>
-      <c r="S28" s="25">
+      <c r="S28" s="20">
         <v>245</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="N18:R18"/>
     <mergeCell ref="M5:Q5"/>
     <mergeCell ref="N15:R15"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="N17:R17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Fuerza a mi amigo Leal
</commit_message>
<xml_diff>
--- a/Array Merge.xlsx
+++ b/Array Merge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\solid\Desktop\ITC\Semestre3\Estructura Datos\Parcial4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B276A035-B102-4B49-BC04-7A0A8F7736A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74269E9-5777-4977-91DD-82E0706C4145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="3700" windowWidth="7500" windowHeight="6000" xr2:uid="{D027E261-0996-4E73-9EA8-3C78A974A5B2}"/>
+    <workbookView xWindow="9280" yWindow="2420" windowWidth="7500" windowHeight="6000" xr2:uid="{D027E261-0996-4E73-9EA8-3C78A974A5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>i</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Lim Index grupo = 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j </t>
   </si>
 </sst>
 </file>
@@ -71,7 +74,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,14 +99,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -268,11 +265,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,11 +335,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -335,21 +349,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,9 +385,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FFFF9999"/>
-      <color rgb="FFCCFFCC"/>
-      <color rgb="FFCCFFFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -673,14 +700,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1F7E58-B7CD-4169-A9E1-085807763DA9}">
   <dimension ref="C1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="18" width="5.81640625" customWidth="1"/>
-    <col min="19" max="19" width="6" style="19" customWidth="1"/>
+    <col min="19" max="19" width="6" style="33" customWidth="1"/>
     <col min="20" max="20" width="6.1796875" customWidth="1"/>
     <col min="21" max="21" width="6" customWidth="1"/>
     <col min="22" max="37" width="7.36328125" customWidth="1"/>
@@ -736,55 +763,55 @@
       <c r="R2" s="7">
         <v>65</v>
       </c>
-      <c r="S2" s="20">
-        <v>245</v>
-      </c>
-      <c r="V2" s="32">
+      <c r="S2" s="34">
+        <v>13</v>
+      </c>
+      <c r="V2" s="28">
         <v>206</v>
       </c>
-      <c r="W2" s="33">
+      <c r="W2" s="29">
         <v>298</v>
       </c>
-      <c r="X2" s="33">
+      <c r="X2" s="29">
         <v>61</v>
       </c>
-      <c r="Y2" s="33">
+      <c r="Y2" s="29">
         <v>68</v>
       </c>
-      <c r="Z2" s="33">
+      <c r="Z2" s="29">
         <v>117</v>
       </c>
-      <c r="AA2" s="33">
+      <c r="AA2" s="29">
         <v>157</v>
       </c>
-      <c r="AB2" s="33">
+      <c r="AB2" s="29">
         <v>229</v>
       </c>
-      <c r="AC2" s="33">
+      <c r="AC2" s="29">
         <v>63</v>
       </c>
-      <c r="AD2" s="33">
+      <c r="AD2" s="29">
         <v>288</v>
       </c>
-      <c r="AE2" s="33">
+      <c r="AE2" s="29">
         <v>184</v>
       </c>
-      <c r="AF2" s="33">
+      <c r="AF2" s="29">
         <v>250</v>
       </c>
-      <c r="AG2" s="33">
+      <c r="AG2" s="29">
         <v>218</v>
       </c>
-      <c r="AH2" s="33">
+      <c r="AH2" s="29">
         <v>90</v>
       </c>
-      <c r="AI2" s="33">
+      <c r="AI2" s="29">
         <v>296</v>
       </c>
-      <c r="AJ2" s="33">
+      <c r="AJ2" s="29">
         <v>120</v>
       </c>
-      <c r="AK2" s="34">
+      <c r="AK2" s="30">
         <v>65</v>
       </c>
     </row>
@@ -813,6 +840,33 @@
       <c r="J3" s="18">
         <v>7</v>
       </c>
+      <c r="K3" s="27">
+        <v>8</v>
+      </c>
+      <c r="L3" s="27">
+        <v>9</v>
+      </c>
+      <c r="M3" s="27">
+        <v>10</v>
+      </c>
+      <c r="N3" s="27">
+        <v>11</v>
+      </c>
+      <c r="O3" s="27">
+        <v>12</v>
+      </c>
+      <c r="P3" s="27">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>14</v>
+      </c>
+      <c r="R3" s="27">
+        <v>15</v>
+      </c>
+      <c r="S3" s="27">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J4" t="s">
@@ -820,65 +874,65 @@
       </c>
     </row>
     <row r="5" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="22">
+      <c r="C5" s="19">
         <v>206</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="19">
         <v>61</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="19">
         <v>117</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="21">
         <v>229</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="21">
         <v>288</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="21">
         <v>250</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="21">
         <v>90</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="21">
         <v>120</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
     </row>
     <row r="6" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" s="31" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
     </row>
     <row r="7" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="22">
+      <c r="C7" s="19">
         <v>298</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="19">
         <v>68</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="19">
         <v>157</v>
       </c>
       <c r="F7" s="14">
@@ -896,15 +950,18 @@
       <c r="J7" s="14">
         <v>65</v>
       </c>
+      <c r="K7" s="21">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D8" s="27"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="2">
         <v>206</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="23">
         <v>298</v>
       </c>
       <c r="E9" s="3">
@@ -943,10 +1000,14 @@
       <c r="P9" s="3">
         <v>296</v>
       </c>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="20">
-        <v>245</v>
+      <c r="Q9" s="3">
+        <v>13</v>
+      </c>
+      <c r="R9" s="3">
+        <v>65</v>
+      </c>
+      <c r="S9" s="12">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -994,13 +1055,13 @@
         <v>296</v>
       </c>
       <c r="Q13" s="7">
+        <v>13</v>
+      </c>
+      <c r="R13" s="7">
         <v>65</v>
       </c>
-      <c r="R13" s="7">
+      <c r="S13" s="34">
         <v>120</v>
-      </c>
-      <c r="S13" s="20">
-        <v>245</v>
       </c>
     </row>
     <row r="15" spans="3:37" x14ac:dyDescent="0.35">
@@ -1016,22 +1077,26 @@
       <c r="F15" s="1">
         <v>3</v>
       </c>
-      <c r="G15" s="29"/>
+      <c r="G15" s="26">
+        <v>4</v>
+      </c>
       <c r="H15" s="1">
         <v>5</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="26">
+        <v>6</v>
+      </c>
       <c r="J15" s="1">
         <v>7</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="26">
         <v>8</v>
       </c>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
     </row>
     <row r="16" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G16" t="s">
@@ -1067,13 +1132,13 @@
         <v>296</v>
       </c>
       <c r="L17" s="15"/>
-      <c r="N17" s="31" t="s">
+      <c r="N17" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
     </row>
     <row r="18" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="10"/>
@@ -1088,17 +1153,18 @@
         <v>1</v>
       </c>
       <c r="J18" s="11"/>
+      <c r="K18" s="38"/>
       <c r="L18" s="11"/>
-      <c r="N18" s="30" t="s">
+      <c r="N18" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
     </row>
     <row r="19" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="28">
+      <c r="C19" s="25">
         <v>61</v>
       </c>
       <c r="D19" s="8">
@@ -1117,9 +1183,12 @@
         <v>250</v>
       </c>
       <c r="I19" s="9">
+        <v>13</v>
+      </c>
+      <c r="J19" s="8">
         <v>65</v>
       </c>
-      <c r="J19" s="12">
+      <c r="K19" s="37">
         <v>120</v>
       </c>
       <c r="L19" s="16"/>
@@ -1162,12 +1231,20 @@
       <c r="N22" s="6">
         <v>288</v>
       </c>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="20">
-        <v>245</v>
+      <c r="O22" s="7">
+        <v>13</v>
+      </c>
+      <c r="P22" s="7">
+        <v>65</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>90</v>
+      </c>
+      <c r="R22" s="7">
+        <v>120</v>
+      </c>
+      <c r="S22" s="34">
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1197,85 +1274,85 @@
         <v>298</v>
       </c>
       <c r="K25" s="17">
+        <v>13</v>
+      </c>
+      <c r="L25" s="17">
         <v>65</v>
       </c>
-      <c r="L25" s="17">
+      <c r="M25" s="17">
         <v>90</v>
       </c>
-      <c r="M25" s="17">
+      <c r="N25" s="17">
         <v>120</v>
       </c>
-      <c r="N25" s="17">
+      <c r="O25" s="17">
         <v>184</v>
       </c>
-      <c r="O25" s="17">
+      <c r="P25" s="17">
         <v>218</v>
       </c>
-      <c r="P25" s="17">
+      <c r="Q25" s="17">
         <v>250</v>
       </c>
-      <c r="Q25" s="17">
+      <c r="R25" s="17">
         <v>288</v>
       </c>
-      <c r="R25" s="17">
+      <c r="S25" s="35">
         <v>296</v>
-      </c>
-      <c r="S25" s="21">
-        <v>245</v>
       </c>
     </row>
     <row r="27" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="28" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="5">
+        <v>13</v>
+      </c>
+      <c r="D28" s="6">
         <v>61</v>
       </c>
-      <c r="D28" s="6">
+      <c r="E28" s="6">
         <v>63</v>
       </c>
-      <c r="E28" s="6">
+      <c r="F28" s="6">
         <v>65</v>
       </c>
-      <c r="F28" s="6">
+      <c r="G28" s="6">
         <v>68</v>
       </c>
-      <c r="G28" s="6">
+      <c r="H28" s="6">
         <v>90</v>
       </c>
-      <c r="H28" s="6">
+      <c r="I28" s="6">
         <v>117</v>
       </c>
-      <c r="I28" s="6">
+      <c r="J28" s="6">
         <v>120</v>
       </c>
-      <c r="J28" s="6">
+      <c r="K28" s="6">
         <v>157</v>
       </c>
-      <c r="K28" s="6">
+      <c r="L28" s="6">
         <v>184</v>
       </c>
-      <c r="L28" s="6">
+      <c r="M28" s="6">
         <v>206</v>
       </c>
-      <c r="M28" s="6">
+      <c r="N28" s="6">
         <v>218</v>
       </c>
-      <c r="N28" s="6">
+      <c r="O28" s="6">
         <v>229</v>
       </c>
-      <c r="O28" s="6">
+      <c r="P28" s="6">
         <v>250</v>
       </c>
-      <c r="P28" s="6">
+      <c r="Q28" s="6">
         <v>288</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="R28" s="6">
         <v>296</v>
       </c>
-      <c r="R28" s="6">
+      <c r="S28" s="36">
         <v>298</v>
-      </c>
-      <c r="S28" s="20">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>